<commit_message>
update trans to the output. bugs fixed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,33 +14,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>c_office_id</t>
   </si>
   <si>
+    <t>c_office_chn</t>
+  </si>
+  <si>
     <t>c_dy</t>
   </si>
   <si>
+    <t>c_office_trans</t>
+  </si>
+  <si>
     <t>c_office_pinyin</t>
   </si>
   <si>
-    <t>c_office_chn</t>
-  </si>
-  <si>
     <t>c_source</t>
   </si>
   <si>
+    <t>僧錄司</t>
+  </si>
+  <si>
+    <t>僧錄司善世</t>
+  </si>
+  <si>
+    <t>僧錄司左善世</t>
+  </si>
+  <si>
+    <t>僧錄司右善世</t>
+  </si>
+  <si>
+    <t>僧錄司闡教</t>
+  </si>
+  <si>
+    <t>僧錄司左闡教</t>
+  </si>
+  <si>
+    <t>僧錄司右闡教</t>
+  </si>
+  <si>
+    <t>僧錄司講經</t>
+  </si>
+  <si>
+    <t>僧錄司左講經</t>
+  </si>
+  <si>
+    <t>僧錄司右講經</t>
+  </si>
+  <si>
+    <t>僧錄司覺義</t>
+  </si>
+  <si>
+    <t>僧錄司左覺義</t>
+  </si>
+  <si>
+    <t>僧錄司右覺義</t>
+  </si>
+  <si>
+    <t>府學訓導</t>
+  </si>
+  <si>
     <t>19</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>The Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Buddhist Patriarch of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Left Buddhist Patriarch of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Right Buddhist Patriarch of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Supervisory Monk for Buddhist Practices of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Left Supervisory Monk for Buddhist Practices of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Right Supervisory Monk for Buddhist Practices of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Lecturing Monk of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Left Lecturing Monk of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Right Lecturing Monk of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Buddhist Rectifier of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Left Buddhist Rectifier of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Right Buddhist Rectifier of the Central Buddhist Registry</t>
+  </si>
+  <si>
+    <t>Assistant Instructor in a Prefectural Confucian School</t>
+  </si>
+  <si>
     <t>seng lu si</t>
   </si>
   <si>
-    <t>僧錄司</t>
+    <t>seng lu si shan shi</t>
+  </si>
+  <si>
+    <t>seng lu si zuo shan shi</t>
+  </si>
+  <si>
+    <t>seng lu si you shan shi</t>
+  </si>
+  <si>
+    <t>seng lu si chan jiao</t>
+  </si>
+  <si>
+    <t>seng lu si zuo chan jiao</t>
+  </si>
+  <si>
+    <t>seng lu si you chan jiao</t>
+  </si>
+  <si>
+    <t>seng lu si jiang jing</t>
+  </si>
+  <si>
+    <t>seng lu si zuo jiang jing</t>
+  </si>
+  <si>
+    <t>seng lu si you jiang jing</t>
+  </si>
+  <si>
+    <t>seng lu si jue yi</t>
+  </si>
+  <si>
+    <t>seng lu si zuo jue yi</t>
+  </si>
+  <si>
+    <t>seng lu si you jue yi</t>
+  </si>
+  <si>
+    <t>fu xue xun dao</t>
   </si>
   <si>
     <t>18417</t>
+  </si>
+  <si>
+    <t>65006</t>
   </si>
 </sst>
 </file>
@@ -398,13 +527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,22 +549,288 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>802012</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>802013</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>802014</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>802015</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>802016</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>802017</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>802018</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>802019</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>802020</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>802021</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>802022</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>802023</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>802024</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>802025</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update new official titles
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>c_office_id</t>
   </si>
@@ -34,9 +34,6 @@
     <t>c_source</t>
   </si>
   <si>
-    <t>南京水軍左衞</t>
-  </si>
-  <si>
     <t>鑄印局大使</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>Left Guard of Nanking Navy</t>
-  </si>
-  <si>
     <t>Commissioner of Seals Service</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
   </si>
   <si>
     <t>One of Prestige Titles (Civil)（Rank 8 ，upper class，lower grade）</t>
-  </si>
-  <si>
-    <t>nan jing shui jun zuo wei</t>
   </si>
   <si>
     <t>zhu yin ju da shi</t>
@@ -443,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,16 +468,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -500,13 +491,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -520,33 +511,13 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>802052</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create new official titles
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>c_office_id</t>
   </si>
@@ -34,49 +34,19 @@
     <t>c_source</t>
   </si>
   <si>
-    <t>鑄印局大使</t>
-  </si>
-  <si>
-    <t>判三司戶部理欠司</t>
-  </si>
-  <si>
-    <t>徵事郎</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Commissioner of Seals Service</t>
-  </si>
-  <si>
-    <t>Supervisor of the Deficits Monitoring Office of the Census Bureau in the State Finance Commission</t>
-  </si>
-  <si>
-    <t>One of Prestige Titles (Civil)（Rank 8 ，upper class，lower grade）</t>
-  </si>
-  <si>
-    <t>zhu yin ju da shi</t>
-  </si>
-  <si>
-    <t>pan san si hu bu li qian si</t>
-  </si>
-  <si>
-    <t>zheng shi lang</t>
+    <t>宣慰使司都元帥府參謀</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Counselor of the Chief Military Command</t>
+  </si>
+  <si>
+    <t>xuan wei shi si dou yuan shuai fu can mou</t>
   </si>
   <si>
     <t>2067</t>
-  </si>
-  <si>
-    <t>2229</t>
-  </si>
-  <si>
-    <t>24844</t>
   </si>
 </sst>
 </file>
@@ -434,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,62 +432,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>802049</v>
+        <v>803728</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>802050</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>802051</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create new official title
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -34,19 +34,19 @@
     <t>c_source</t>
   </si>
   <si>
-    <t>宣慰使司都元帥府參謀</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Counselor of the Chief Military Command</t>
-  </si>
-  <si>
-    <t>xuan wei shi si dou yuan shuai fu can mou</t>
-  </si>
-  <si>
-    <t>2067</t>
+    <t>送伴使</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Parting Commissioner（Tackett）</t>
+  </si>
+  <si>
+    <t>song ban shi</t>
+  </si>
+  <si>
+    <t>66675</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>803728</v>
+        <v>803734</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
create new office titles
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,61 +467,91 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>803737</v>
+        <v>803739</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>國史實錄院校勘</t>
+          <t>直御書處</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Unranked Subofficials attached to the Historiography and True Records Institute</t>
+          <t>Auxiliary in the Imperial Library</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>guo shi shi lu yuan jiao kan</t>
+          <t>zhi yu shu chu</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2229</t>
+          <t>17477</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>803738</v>
+        <v>803740</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>諸王宮伴讀</t>
+          <t>提學副使</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Reader-companion of Princely Palaces</t>
+          <t>Vice Commissioner of an Education Intendant Circuit</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>zhu wang gong ban du</t>
+          <t>ti xue fu shi</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>64847</t>
+          <t>2067</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>803741</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>世職一等阿達哈哈番</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Hereditary Title of Commandant of Light Chariots</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>shi zhi yi deng a da ha ha fan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2067</t>
         </is>
       </c>
     </row>

</xml_diff>